<commit_message>
Fixed quest message grammatical errors (related to each item), and updated the excel sheet to the completed version.
</commit_message>
<xml_diff>
--- a/Assets/Scripts/Quests.xlsx
+++ b/Assets/Scripts/Quests.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\ldjam48\Assets\Scripts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UnityGames\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E88B4B32-978C-4801-94D7-9927A4E2900D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372"/>
   </bookViews>
   <sheets>
     <sheet name="Quests" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="312">
   <si>
     <t>Success</t>
   </si>
@@ -61,15 +60,9 @@
     <t>You're a hard worker. Looks like your tools broke though. Sorry.</t>
   </si>
   <si>
-    <t>Not sure how you did all that tilling with [item], but I'm grateful.</t>
-  </si>
-  <si>
     <t>You're a hard worker, good with your hands.</t>
   </si>
   <si>
-    <t>Why'd you think you could till a field with [item]? And now it's all dirty and messed up.</t>
-  </si>
-  <si>
     <t>This work isn't easy without the right tools. I thought you would have your own. Maybe try helping some other people.</t>
   </si>
   <si>
@@ -85,15 +78,9 @@
     <t xml:space="preserve">Looks like you went a bit overboard and broke those tools! Fields are done though, thank you. </t>
   </si>
   <si>
-    <t>Not sure how you did all that planting with [item], but I'm grateful.</t>
-  </si>
-  <si>
     <t>All that planting by hand! Good on you.</t>
   </si>
   <si>
-    <t>Why'd you think you could plant seeds with [item]? And now it's all dirty and messed up.</t>
-  </si>
-  <si>
     <t>Planting isn't easy without the right tools. I thought you would have your own. Maybe try helping some other people.</t>
   </si>
   <si>
@@ -106,18 +93,9 @@
     <t>Seeds, Hoe, Shovel, Garden Fork, Trowel</t>
   </si>
   <si>
-    <t>Thank you, and so thoughtful to bring [item] for me.</t>
-  </si>
-  <si>
-    <t>Thank you for your help! I don't know why you brought [item] with, but thank you for that too.</t>
-  </si>
-  <si>
     <t>Thank you for your help!</t>
   </si>
   <si>
-    <t>Oh I suppose you can't use [item] to plant seeds.</t>
-  </si>
-  <si>
     <t>Oh it seems this work might be too much for you. Perhaps if you had some tools to help?</t>
   </si>
   <si>
@@ -133,15 +111,9 @@
     <t xml:space="preserve">Good harvest. Glad you brought tools with. </t>
   </si>
   <si>
-    <t>Good harvest. Weird that you used [item]. I wouldn't have.</t>
-  </si>
-  <si>
     <t>Good harvest. Just working with your hands.</t>
   </si>
   <si>
-    <t>You weren't much help out there; maybe because [item] isn't the right tool.</t>
-  </si>
-  <si>
     <t>Not much help out there, maybe if you had some tools of your own.</t>
   </si>
   <si>
@@ -157,15 +129,9 @@
     <t>Quite a few rocks. Thank you kindly for your work.</t>
   </si>
   <si>
-    <t>Thank you kindly. Impressive how you used that [item] today.</t>
-  </si>
-  <si>
     <t>Thank you kindly. Hope your hands don't hurt too bad.</t>
   </si>
   <si>
-    <t>You left a lot of rocks behind. Maybe because you don't use [item] to dig up rocks?</t>
-  </si>
-  <si>
     <t>Looks like your hands got real beat up. Sometimes you just can't do it by hand.</t>
   </si>
   <si>
@@ -187,9 +153,6 @@
     <t>Thank you! You say you cupped your hands to move the water to the plants? Oh. Well, it worked.</t>
   </si>
   <si>
-    <t>Ah. The fields look a bit dry. Maybe if you had a watering can instead of [item]?</t>
-  </si>
-  <si>
     <t>Ah. The fields look a bit dry. Maybe if you had a watering can instead of cupping your hands?</t>
   </si>
   <si>
@@ -205,15 +168,9 @@
     <t>Thank you so much! Sorry you had to bring your own supplies.</t>
   </si>
   <si>
-    <t>Thank you! I have no clue how you did that with [item], but thank you!</t>
-  </si>
-  <si>
     <t xml:space="preserve">Thank you!  </t>
   </si>
   <si>
-    <t>Oh. This food isn't very good. Maybe you shouldn't cook with [item].</t>
-  </si>
-  <si>
     <t>Oh. This food isn't very good. I think we need some more kitchen tools.</t>
   </si>
   <si>
@@ -226,18 +183,9 @@
     <t>Bucket, Paintbrush</t>
   </si>
   <si>
-    <t>That was fun, right? And thanks for the [item]!</t>
-  </si>
-  <si>
-    <t>Fun, right? Weird that you used [item] to paint though.</t>
-  </si>
-  <si>
     <t>Fun, right?</t>
   </si>
   <si>
-    <t>Guess I need to do this myself. You can't paint with [item].</t>
-  </si>
-  <si>
     <t>Guess I need to do this myself. You can't paint without a brush.</t>
   </si>
   <si>
@@ -259,9 +207,6 @@
     <t>Wow, I can't believe he ran up to you like that!</t>
   </si>
   <si>
-    <t>Oh…he ran away from you. Maybe he was afraid of the [item]?</t>
-  </si>
-  <si>
     <t>Oh…he ran away from you. I guess I should have expected that.</t>
   </si>
   <si>
@@ -277,15 +222,9 @@
     <t>Wow! You're fast. Kinda ruined your shoes. Sorry.</t>
   </si>
   <si>
-    <t>Wow. You're fast! What's with the [item]?</t>
-  </si>
-  <si>
     <t>Wow! You're fast.</t>
   </si>
   <si>
-    <t>Not fast enough for me, sorry. What's with the [item]?</t>
-  </si>
-  <si>
     <t>Really Big Fish</t>
   </si>
   <si>
@@ -472,45 +411,21 @@
     <t>Dripping! There's a dripping from underneath my floorboards! A tell-tale sign of water damage. Help me find the leak?</t>
   </si>
   <si>
-    <t>I knew it was real! Good thing you had that [item].</t>
-  </si>
-  <si>
-    <t>I knew it was real! But…I don't want to know what you used that [item] for.</t>
-  </si>
-  <si>
     <t>I knew it was real! And you caught it barehanded? Amazing!</t>
   </si>
   <si>
-    <t>What's [item] for? You didn't find the fish?</t>
-  </si>
-  <si>
     <t>You couldn't find it either? Aw man.</t>
   </si>
   <si>
-    <t>I guess the kids liked [item]! Thank you.</t>
-  </si>
-  <si>
     <t>Wow, you're great with kids!</t>
   </si>
   <si>
-    <t xml:space="preserve">My kids didn't seem to like [item]. </t>
-  </si>
-  <si>
     <t>You aren't very good with kids, are you.</t>
   </si>
   <si>
-    <t>Yippee! We caught so many frogs in that [item].</t>
-  </si>
-  <si>
-    <t>Yippee! You caught so many frogs with…[item]?</t>
-  </si>
-  <si>
     <t>You caught so many frogs with just your hands!</t>
   </si>
   <si>
-    <t>Aw, you didn't catch very many frogs. I don't see how you would with [item].</t>
-  </si>
-  <si>
     <t>Aw, you didn't get very many.</t>
   </si>
   <si>
@@ -523,81 +438,45 @@
     <t>Net</t>
   </si>
   <si>
-    <t>Oh wow! They're so beautiful, you're good with [item].</t>
-  </si>
-  <si>
-    <t>Oh wow, they're beautiful! And you caught them with [item]?</t>
-  </si>
-  <si>
     <t>Oh wow, they're so lovely! And they just landed on you?</t>
   </si>
   <si>
-    <t>Oh no, you didn't catch any? Using…[item]…</t>
-  </si>
-  <si>
     <t>Oh no, the butterflies don't really like you.</t>
   </si>
   <si>
     <t>Bucket, Shovel, Trowel</t>
   </si>
   <si>
-    <t>Wiggly! Wriggly! Squirmy! Wormy! You're good with [item].</t>
-  </si>
-  <si>
-    <t>Wiggly! Wriggly! Squirmy! Wormy! How'd you get so many worms with [item]?</t>
-  </si>
-  <si>
     <t>Wiggly! Wriggly! Squirmy! Wormy! How'd you get so many worms with just your hands?</t>
   </si>
   <si>
-    <t>No worms? Why do you have [item]?</t>
-  </si>
-  <si>
     <t>No worms today? Maybe we need a shovel.</t>
   </si>
   <si>
     <t>I'll do some good fishing with these. Thank you.</t>
   </si>
   <si>
-    <t>Not sure how you pulled it off with [item], but I won't complain. Thank you.</t>
-  </si>
-  <si>
     <t>You caught those worms barehanded? Good for you.</t>
   </si>
   <si>
-    <t>No worms? Maybe you shouldn't use [item]?</t>
-  </si>
-  <si>
     <t>No worms? Maybe try a shovel next time.</t>
   </si>
   <si>
     <t>Ah! Marvelous. Thank you.</t>
   </si>
   <si>
-    <t>Ah! Wonderful, though, what is [item] for?</t>
-  </si>
-  <si>
     <t>Ah! Wonderful, and you caught them…with your hands?</t>
   </si>
   <si>
-    <t>Ah, no luck? Perhaps [item] isn't the tool you needed.</t>
-  </si>
-  <si>
     <t>Ah, no luck? Perhaps a butterfly net would have helped.</t>
   </si>
   <si>
     <t>Oh! Wonderful specimens. My thanks.</t>
   </si>
   <si>
-    <t>Ah! Glorious, and you used [item] to catch them?</t>
-  </si>
-  <si>
     <t>Oh! You captured them barehanded? Very good.</t>
   </si>
   <si>
-    <t>You couldn't find any? Perhaps it's because you were using [item].</t>
-  </si>
-  <si>
     <t>No frogs? They are quite slippery, barehanded is oft not the best approach.</t>
   </si>
   <si>
@@ -607,15 +486,9 @@
     <t>Thank you thank you! Though, I'm sorry the birds ruined your [item]. Not too scary I suppose.</t>
   </si>
   <si>
-    <t>Thank you! [item] was a nice touch.</t>
-  </si>
-  <si>
     <t>Thank you! You must be terrifying. (To birds).</t>
   </si>
   <si>
-    <t>Oh there are birds everywhere! I suppose [item] can't scare them.</t>
-  </si>
-  <si>
     <t>Oh there are birds everywhere! Maybe if you had something else to help you scare them.</t>
   </si>
   <si>
@@ -625,15 +498,9 @@
     <t>That was a good aventure! Your exploring items were very helpful.</t>
   </si>
   <si>
-    <t>That was a good adventure! [item] didn't seem particularly helpful though.</t>
-  </si>
-  <si>
     <t>That was a good adventure!</t>
   </si>
   <si>
-    <t>That wasn't very fun. I think it's because you brought [item].</t>
-  </si>
-  <si>
     <t>That wasn't very fun. You should have brought something fun.</t>
   </si>
   <si>
@@ -646,30 +513,18 @@
     <t>It's beautiful!</t>
   </si>
   <si>
-    <t>You're great with [item]. Not sure how you pulled it off though.</t>
-  </si>
-  <si>
     <t>You sure are good with your hands.</t>
   </si>
   <si>
-    <t>Oh no, this is not going well. Why are you using [item]?</t>
-  </si>
-  <si>
     <t>Oh no, this isn't good. I guess we should have used tools.</t>
   </si>
   <si>
     <t>This was so much better with you here.</t>
   </si>
   <si>
-    <t>This went so quickly! Even if you did paint with [item].</t>
-  </si>
-  <si>
     <t>You can really paint!</t>
   </si>
   <si>
-    <t>There's paint everywhere! Why did you use [item] instead of a paintbrush?</t>
-  </si>
-  <si>
     <t>I think this would have gone better if we had a bucket for the paint.</t>
   </si>
   <si>
@@ -694,9 +549,6 @@
     <t>Corn, Net</t>
   </si>
   <si>
-    <t>Good thinking with that [item]!</t>
-  </si>
-  <si>
     <t>Not sure how your [item] came into play, but my chickens are back!</t>
   </si>
   <si>
@@ -712,19 +564,403 @@
     <t>It's gone? You swear? Thank you!</t>
   </si>
   <si>
-    <t>Bucket, Net, Shoes</t>
-  </si>
-  <si>
     <t>You smacked it? EW! I mean, thank you.</t>
   </si>
   <si>
     <t>WHY DID YOU GO IN THERE WITH YOUR [item]????</t>
+  </si>
+  <si>
+    <t>Oh thank you!</t>
+  </si>
+  <si>
+    <t>You used your HANDS? …thank you</t>
+  </si>
+  <si>
+    <t>Oh no! Why did you use your [item]? That didn't work at all!</t>
+  </si>
+  <si>
+    <t>You tried using your hands? Of course that didn't work!</t>
+  </si>
+  <si>
+    <t>Bucket, Net</t>
+  </si>
+  <si>
+    <t>Bucket, Net, Shoes, Shovel</t>
+  </si>
+  <si>
+    <t>You wore out your shoes delivering them? Wow, glad I didn't do it!</t>
+  </si>
+  <si>
+    <t>What do you mean you used your [item] to deliver them? I can't complain about the results though.</t>
+  </si>
+  <si>
+    <t>That's some good mailing!</t>
+  </si>
+  <si>
+    <t>How were you going to use your [item] to deliver them? It didn't work though…</t>
+  </si>
+  <si>
+    <t>Couldn't hack it? Well. Okay I guess.</t>
+  </si>
+  <si>
+    <t>Shoes, Shirt, Hat, Pants</t>
+  </si>
+  <si>
+    <t>Oh cool [item]. I think everyone liked that.</t>
+  </si>
+  <si>
+    <t>Oh cool. People liked your…[item], I think.</t>
+  </si>
+  <si>
+    <t>You are so cool! Now I'm cool!</t>
+  </si>
+  <si>
+    <t>I think your [item] made people not like me.</t>
+  </si>
+  <si>
+    <t>I think we're both unpopular now.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Steak </t>
+  </si>
+  <si>
+    <t>That was great!</t>
+  </si>
+  <si>
+    <t>I didn't think they would like your [item], but it worked out!</t>
+  </si>
+  <si>
+    <t>You're really good at this.</t>
+  </si>
+  <si>
+    <t>I think your [item] made things weird.</t>
+  </si>
+  <si>
+    <t>I don't think you're up for this.</t>
+  </si>
+  <si>
+    <t>Pants, Steak, Chicken</t>
+  </si>
+  <si>
+    <t>GLORIOUS.</t>
+  </si>
+  <si>
+    <t>EXCELLENT. YOUR [item] MADE THINGS INTERESTING.</t>
+  </si>
+  <si>
+    <t>YOU ARE A WONDERFUL SPECIMEN.</t>
+  </si>
+  <si>
+    <t>YOUR [item] WAS NOT APPROPRIATE HERE.</t>
+  </si>
+  <si>
+    <t>YOU ARE NOT A CHALLENGE FOR ME.</t>
+  </si>
+  <si>
+    <t>Basket, Bucket</t>
+  </si>
+  <si>
+    <t>I'm going to the bathroom right away! Thank you!</t>
+  </si>
+  <si>
+    <t>I love your outfit! And a good dancer too.</t>
+  </si>
+  <si>
+    <t>Oh you're very good! I think I'll be ready, come festival time.</t>
+  </si>
+  <si>
+    <t>Oh! Your [item] threw me off, but you're quite good.</t>
+  </si>
+  <si>
+    <t>Oh, your [item] seems to be getting in the way of our dancing.</t>
+  </si>
+  <si>
+    <t>You aren't a good dancer, are you?</t>
+  </si>
+  <si>
+    <t>Really making a splash with your [item]. Wonderful!</t>
+  </si>
+  <si>
+    <t>This will be fun!</t>
+  </si>
+  <si>
+    <t>I don't think this will work, me, and you, and your [item].</t>
+  </si>
+  <si>
+    <t>Oh. Maybe I'll go alone.</t>
+  </si>
+  <si>
+    <t>Shovel, Bucket, Trowel</t>
+  </si>
+  <si>
+    <t>Ha! Haha! No more holes! No more holes!</t>
+  </si>
+  <si>
+    <t>Ha! Haha! So many holes! So many holes!</t>
+  </si>
+  <si>
+    <t>How did you fill those holes with your [item]? Erm, I mean, thank you.</t>
+  </si>
+  <si>
+    <t>You used your HANDS? WONDERFUL!</t>
+  </si>
+  <si>
+    <t>Good. Good. Impressive digging with your [item].</t>
+  </si>
+  <si>
+    <t>Shovel, Bucket, Trowel, Hoe</t>
+  </si>
+  <si>
+    <t>Holes! There are still holes! Why were you using your [item]?</t>
+  </si>
+  <si>
+    <t>Holes! There are still holes! Why are you using your hands?</t>
+  </si>
+  <si>
+    <t>Holes…Where are the holes? You can't dig with your [item].</t>
+  </si>
+  <si>
+    <t>Holes…Where are the holes? You can't dig with your hands.</t>
+  </si>
+  <si>
+    <t>Trowel, Shovel, Bucket</t>
+  </si>
+  <si>
+    <t>Mushroom Mushroom Mushroom! Let's go again sometime.</t>
+  </si>
+  <si>
+    <t>Oh, a strange technique there, finding mushrooms with your [item]. But successful nonetheless!</t>
+  </si>
+  <si>
+    <t>You sniff out mushrooms with your…nose? Incredible.</t>
+  </si>
+  <si>
+    <t>No mushrooms? Perhaps using your [item] was not a good idea.</t>
+  </si>
+  <si>
+    <t>Nor very many mushrooms. They can be hard to find.</t>
+  </si>
+  <si>
+    <t>Not sure about your [item], but you can sing!</t>
+  </si>
+  <si>
+    <t>Wow, you can sing! That makes one of us!</t>
+  </si>
+  <si>
+    <t>We we're kind of destined to fail. Making a big deal of your [item] made it weird though.</t>
+  </si>
+  <si>
+    <t>Kind of destined to fail, but we did it together!</t>
+  </si>
+  <si>
+    <t>And what was your [item] for again? Anyway, thank you.</t>
+  </si>
+  <si>
+    <t>You're quick! Thank you.</t>
+  </si>
+  <si>
+    <t>You can't catch arrows with your [item]! That's a terrible idea!</t>
+  </si>
+  <si>
+    <t>Shoes, Basket</t>
+  </si>
+  <si>
+    <t>I can practice so much faster now! Thank you.</t>
+  </si>
+  <si>
+    <t>I'm so sorry! Honestly, I've never shot someone before.</t>
+  </si>
+  <si>
+    <t>Bucket</t>
+  </si>
+  <si>
+    <t>Ah! A bucket. Yes, good. Thank you. Yes.</t>
+  </si>
+  <si>
+    <t>Ah! Aha! Quick thinking using your [item] like that. Yes. Yes that will work.</t>
+  </si>
+  <si>
+    <t>Oh, was that all? Thank you, very good.</t>
+  </si>
+  <si>
+    <t>You can't use your [item] to fix a leak! Are you mad! Well, are you!?</t>
+  </si>
+  <si>
+    <t>You've come empty handed! How are we to fix this leak? How!</t>
+  </si>
+  <si>
+    <t>Net, Basket</t>
+  </si>
+  <si>
+    <t>It's so pristine! Oh thank you, thank you.</t>
+  </si>
+  <si>
+    <t>I didn't think your [item] would help, but it has! Fantastic.</t>
+  </si>
+  <si>
+    <t>You caught it bare handed? Impressive!</t>
+  </si>
+  <si>
+    <t>It ran away? Well how did you think your [item] would help?</t>
+  </si>
+  <si>
+    <t>It ran away? Oh, oh I suppose I'll keep looking then.</t>
+  </si>
+  <si>
+    <t>Thank you, and so thoughtful to bring your [item] for me.</t>
+  </si>
+  <si>
+    <t>That was fun, right? And thanks for your [item]!</t>
+  </si>
+  <si>
+    <t>I knew it was real! Good thing you had your [item].</t>
+  </si>
+  <si>
+    <t>Yippee! We caught so many frogs with your [item].</t>
+  </si>
+  <si>
+    <t>Oh wow! They're so beautiful, you're really good with your [item].</t>
+  </si>
+  <si>
+    <t>Wiggly! Wriggly! Squirmy! Wormy! You're good really with your [item].</t>
+  </si>
+  <si>
+    <t>Good thinking with your [item]!</t>
+  </si>
+  <si>
+    <t>Not sure how you did all that tilling with your [item], but I'm grateful.</t>
+  </si>
+  <si>
+    <t>Not sure how you did all that planting with your [item], but I'm grateful.</t>
+  </si>
+  <si>
+    <t>Thank you for your help! I don't know why you brought your [item] with, but thank you for that too.</t>
+  </si>
+  <si>
+    <t>Good harvest. Weird that you used your [item]. I wouldn't have.</t>
+  </si>
+  <si>
+    <t>Thank you kindly. Impressive how you used your [item] today.</t>
+  </si>
+  <si>
+    <t>Thank you! I have no clue how you did that with your [item], but thank you!</t>
+  </si>
+  <si>
+    <t>Fun, right? Weird that you used your [item] to paint though.</t>
+  </si>
+  <si>
+    <t>Wow. You're fast! What's with your [item]?</t>
+  </si>
+  <si>
+    <t>I knew it was real! But…I don't want to know what you used your [item] for.</t>
+  </si>
+  <si>
+    <t>I guess the kids liked your [item]! Thank you.</t>
+  </si>
+  <si>
+    <t>Yippee! You caught so many frogs with…your [item]?</t>
+  </si>
+  <si>
+    <t>Oh wow, they're beautiful! And you caught them with your [item]?</t>
+  </si>
+  <si>
+    <t>Wiggly! Wriggly! Squirmy! Wormy! How'd you get so many worms with your [item]?</t>
+  </si>
+  <si>
+    <t>Not sure how you pulled it off with your [item], but I won't complain. Thank you.</t>
+  </si>
+  <si>
+    <t>Ah! Wonderful, though, what is your [item] for?</t>
+  </si>
+  <si>
+    <t>Ah! Glorious, and you used your [item] to catch them?</t>
+  </si>
+  <si>
+    <t>Thank you! Your [item] was a nice touch.</t>
+  </si>
+  <si>
+    <t>That was a good adventure! Your [item] didn't seem particularly helpful though.</t>
+  </si>
+  <si>
+    <t>You're great with your [item]. Not sure how you pulled it off though.</t>
+  </si>
+  <si>
+    <t>This went so quickly! Even if you did paint with your [item].</t>
+  </si>
+  <si>
+    <t>I wouldn't have used my [item], but I can't complain!</t>
+  </si>
+  <si>
+    <t>There's paint everywhere! Why did you use your [item] instead of a paintbrush?</t>
+  </si>
+  <si>
+    <t>Oh no, this is not going well. Why are you using your [item]?</t>
+  </si>
+  <si>
+    <t>That wasn't very fun. I think it's because you brought your [item].</t>
+  </si>
+  <si>
+    <t>Oh there are birds everywhere! I suppose your [item] can't scare them.</t>
+  </si>
+  <si>
+    <t>You couldn't find any? Perhaps it's because you were using your [item].</t>
+  </si>
+  <si>
+    <t>Ah, no luck? Perhaps your [item] isn't the tool you needed.</t>
+  </si>
+  <si>
+    <t>No worms? Maybe you shouldn't use your [item]?</t>
+  </si>
+  <si>
+    <t>No worms? Why do you have your [item]?</t>
+  </si>
+  <si>
+    <t>Oh no, you didn't catch any? Using…your [item]…</t>
+  </si>
+  <si>
+    <t>Aw, you didn't catch very many frogs. I don't see how you would with your [item].</t>
+  </si>
+  <si>
+    <t xml:space="preserve">My kids didn't seem to like your [item]. </t>
+  </si>
+  <si>
+    <t>What's your [item] for? You didn't find the fish?</t>
+  </si>
+  <si>
+    <t>Not fast enough for me, sorry. What's with your [item]?</t>
+  </si>
+  <si>
+    <t>Oh…he ran away from you. Maybe he was afraid of your [item]?</t>
+  </si>
+  <si>
+    <t>Guess I need to do this myself. You can't paint with your [item].</t>
+  </si>
+  <si>
+    <t>Oh. This food isn't very good. Maybe you shouldn't cook with your [item].</t>
+  </si>
+  <si>
+    <t>Ah. The fields look a bit dry. Maybe if you had a watering can instead of your [item]?</t>
+  </si>
+  <si>
+    <t>You left a lot of rocks behind. Maybe because you don't use your [item] to dig up rocks?</t>
+  </si>
+  <si>
+    <t>You weren't much help out there; maybe because your [item] isn't the right tool.</t>
+  </si>
+  <si>
+    <t>Oh I suppose you can't use your [item] to plant seeds.</t>
+  </si>
+  <si>
+    <t>Why'd you think you could plant seeds with your [item]? And now it's all dirty and messed up.</t>
+  </si>
+  <si>
+    <t>Why'd you think you could till a field with your [item]? And now it's all dirty and messed up.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1524,22 +1760,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" topLeftCell="H17" workbookViewId="0">
+      <selection activeCell="I46" sqref="I46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" customWidth="1"/>
-    <col min="2" max="2" width="113.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.44140625" customWidth="1"/>
+    <col min="2" max="2" width="110.5546875" customWidth="1"/>
+    <col min="3" max="3" width="35.21875" customWidth="1"/>
+    <col min="4" max="4" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="79.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="83.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="81.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="103.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E1" t="s">
         <v>0</v>
       </c>
@@ -1556,7 +1796,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1585,7 +1825,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1599,754 +1839,1006 @@
         <v>12</v>
       </c>
       <c r="F3" t="s">
+        <v>269</v>
+      </c>
+      <c r="G3" t="s">
         <v>13</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
+        <v>311</v>
+      </c>
+      <c r="I3" t="s">
         <v>14</v>
       </c>
-      <c r="H3" t="s">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>15</v>
       </c>
-      <c r="I3" t="s">
+      <c r="B4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="C4" t="s">
         <v>17</v>
       </c>
-      <c r="B4" t="s">
+      <c r="E4" t="s">
         <v>18</v>
       </c>
-      <c r="C4" t="s">
+      <c r="F4" t="s">
+        <v>270</v>
+      </c>
+      <c r="G4" t="s">
         <v>19</v>
       </c>
-      <c r="E4" t="s">
+      <c r="H4" t="s">
+        <v>310</v>
+      </c>
+      <c r="I4" t="s">
         <v>20</v>
       </c>
-      <c r="F4" t="s">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>21</v>
       </c>
-      <c r="G4" t="s">
+      <c r="B5" t="s">
         <v>22</v>
       </c>
-      <c r="H4" t="s">
+      <c r="C5" t="s">
         <v>23</v>
       </c>
-      <c r="I4" t="s">
+      <c r="E5" t="s">
+        <v>262</v>
+      </c>
+      <c r="F5" t="s">
+        <v>271</v>
+      </c>
+      <c r="G5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="H5" t="s">
+        <v>309</v>
+      </c>
+      <c r="I5" t="s">
         <v>25</v>
       </c>
-      <c r="B5" t="s">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>26</v>
       </c>
-      <c r="C5" t="s">
+      <c r="B6" t="s">
         <v>27</v>
       </c>
-      <c r="E5" t="s">
+      <c r="C6" t="s">
         <v>28</v>
       </c>
-      <c r="F5" t="s">
+      <c r="E6" t="s">
         <v>29</v>
       </c>
-      <c r="G5" t="s">
+      <c r="F6" t="s">
+        <v>272</v>
+      </c>
+      <c r="G6" t="s">
         <v>30</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H6" t="s">
+        <v>308</v>
+      </c>
+      <c r="I6" t="s">
         <v>31</v>
       </c>
-      <c r="I5" t="s">
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B7" t="s">
         <v>33</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C7" t="s">
         <v>34</v>
       </c>
-      <c r="C6" t="s">
+      <c r="E7" t="s">
         <v>35</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F7" t="s">
+        <v>273</v>
+      </c>
+      <c r="G7" t="s">
         <v>36</v>
       </c>
-      <c r="F6" t="s">
+      <c r="H7" t="s">
+        <v>307</v>
+      </c>
+      <c r="I7" t="s">
         <v>37</v>
       </c>
-      <c r="G6" t="s">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>38</v>
       </c>
-      <c r="H6" t="s">
+      <c r="B8" t="s">
         <v>39</v>
       </c>
-      <c r="I6" t="s">
+      <c r="C8" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="E8" t="s">
         <v>41</v>
       </c>
-      <c r="B7" t="s">
+      <c r="F8" t="s">
         <v>42</v>
       </c>
-      <c r="C7" t="s">
+      <c r="G8" t="s">
         <v>43</v>
       </c>
-      <c r="E7" t="s">
+      <c r="H8" t="s">
+        <v>306</v>
+      </c>
+      <c r="I8" t="s">
         <v>44</v>
       </c>
-      <c r="F7" t="s">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>45</v>
       </c>
-      <c r="G7" t="s">
+      <c r="B9" t="s">
         <v>46</v>
       </c>
-      <c r="H7" t="s">
+      <c r="C9" t="s">
         <v>47</v>
       </c>
-      <c r="I7" t="s">
+      <c r="E9" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="F9" t="s">
+        <v>274</v>
+      </c>
+      <c r="G9" t="s">
         <v>49</v>
       </c>
-      <c r="B8" t="s">
+      <c r="H9" t="s">
+        <v>305</v>
+      </c>
+      <c r="I9" t="s">
         <v>50</v>
       </c>
-      <c r="C8" t="s">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>51</v>
       </c>
-      <c r="E8" t="s">
+      <c r="B10" t="s">
         <v>52</v>
       </c>
-      <c r="F8" t="s">
+      <c r="C10" t="s">
         <v>53</v>
       </c>
-      <c r="G8" t="s">
+      <c r="E10" t="s">
+        <v>263</v>
+      </c>
+      <c r="F10" t="s">
+        <v>275</v>
+      </c>
+      <c r="G10" t="s">
         <v>54</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H10" t="s">
+        <v>304</v>
+      </c>
+      <c r="I10" t="s">
         <v>55</v>
       </c>
-      <c r="I8" t="s">
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B11" t="s">
         <v>57</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C11" t="s">
         <v>58</v>
       </c>
-      <c r="C9" t="s">
+      <c r="E11" t="s">
         <v>59</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F11" t="s">
         <v>60</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G11" t="s">
         <v>61</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H11" t="s">
+        <v>303</v>
+      </c>
+      <c r="I11" t="s">
         <v>62</v>
       </c>
-      <c r="H9" t="s">
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>63</v>
       </c>
-      <c r="I9" t="s">
+      <c r="B12" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="C12" t="s">
         <v>65</v>
       </c>
-      <c r="B10" t="s">
+      <c r="E12" t="s">
         <v>66</v>
       </c>
-      <c r="C10" t="s">
+      <c r="F12" t="s">
+        <v>276</v>
+      </c>
+      <c r="G12" t="s">
         <v>67</v>
       </c>
-      <c r="E10" t="s">
+      <c r="H12" t="s">
+        <v>302</v>
+      </c>
+      <c r="I12" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>68</v>
       </c>
-      <c r="F10" t="s">
+      <c r="B13" t="s">
         <v>69</v>
       </c>
-      <c r="G10" t="s">
+      <c r="C13" t="s">
+        <v>137</v>
+      </c>
+      <c r="E13" t="s">
+        <v>264</v>
+      </c>
+      <c r="F13" t="s">
+        <v>277</v>
+      </c>
+      <c r="G13" t="s">
+        <v>130</v>
+      </c>
+      <c r="H13" t="s">
+        <v>301</v>
+      </c>
+      <c r="I13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>70</v>
       </c>
-      <c r="H10" t="s">
+      <c r="B14" t="s">
         <v>71</v>
       </c>
-      <c r="I10" t="s">
+      <c r="F14" t="s">
+        <v>278</v>
+      </c>
+      <c r="G14" t="s">
+        <v>132</v>
+      </c>
+      <c r="H14" t="s">
+        <v>300</v>
+      </c>
+      <c r="I14" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B15" t="s">
         <v>73</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C15" t="s">
+        <v>136</v>
+      </c>
+      <c r="E15" t="s">
+        <v>265</v>
+      </c>
+      <c r="F15" t="s">
+        <v>279</v>
+      </c>
+      <c r="G15" t="s">
+        <v>134</v>
+      </c>
+      <c r="H15" t="s">
+        <v>299</v>
+      </c>
+      <c r="I15" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>74</v>
       </c>
-      <c r="C11" t="s">
+      <c r="B16" t="s">
         <v>75</v>
       </c>
-      <c r="E11" t="s">
+      <c r="C16" t="s">
+        <v>138</v>
+      </c>
+      <c r="E16" t="s">
+        <v>266</v>
+      </c>
+      <c r="F16" t="s">
+        <v>280</v>
+      </c>
+      <c r="G16" t="s">
+        <v>139</v>
+      </c>
+      <c r="H16" t="s">
+        <v>298</v>
+      </c>
+      <c r="I16" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>76</v>
       </c>
-      <c r="F11" t="s">
+      <c r="B17" t="s">
         <v>77</v>
       </c>
-      <c r="G11" t="s">
+      <c r="C17" t="s">
+        <v>141</v>
+      </c>
+      <c r="E17" t="s">
+        <v>267</v>
+      </c>
+      <c r="F17" t="s">
+        <v>281</v>
+      </c>
+      <c r="G17" t="s">
+        <v>142</v>
+      </c>
+      <c r="H17" t="s">
+        <v>297</v>
+      </c>
+      <c r="I17" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>78</v>
       </c>
-      <c r="H11" t="s">
+      <c r="B18" t="s">
         <v>79</v>
       </c>
-      <c r="I11" t="s">
+      <c r="C18" t="s">
+        <v>141</v>
+      </c>
+      <c r="E18" t="s">
+        <v>144</v>
+      </c>
+      <c r="F18" t="s">
+        <v>282</v>
+      </c>
+      <c r="G18" t="s">
+        <v>145</v>
+      </c>
+      <c r="H18" t="s">
+        <v>296</v>
+      </c>
+      <c r="I18" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="B19" t="s">
         <v>81</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C19" t="s">
+        <v>138</v>
+      </c>
+      <c r="E19" t="s">
+        <v>147</v>
+      </c>
+      <c r="F19" t="s">
+        <v>283</v>
+      </c>
+      <c r="G19" t="s">
+        <v>148</v>
+      </c>
+      <c r="H19" t="s">
+        <v>295</v>
+      </c>
+      <c r="I19" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>82</v>
       </c>
-      <c r="C12" t="s">
+      <c r="B20" t="s">
         <v>83</v>
       </c>
-      <c r="E12" t="s">
+      <c r="C20" t="s">
+        <v>136</v>
+      </c>
+      <c r="E20" t="s">
+        <v>150</v>
+      </c>
+      <c r="F20" t="s">
+        <v>284</v>
+      </c>
+      <c r="G20" t="s">
+        <v>151</v>
+      </c>
+      <c r="H20" t="s">
+        <v>294</v>
+      </c>
+      <c r="I20" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>84</v>
       </c>
-      <c r="F12" t="s">
+      <c r="B21" t="s">
         <v>85</v>
       </c>
-      <c r="G12" t="s">
+      <c r="C21" t="s">
+        <v>153</v>
+      </c>
+      <c r="E21" t="s">
+        <v>154</v>
+      </c>
+      <c r="F21" t="s">
+        <v>285</v>
+      </c>
+      <c r="G21" t="s">
+        <v>155</v>
+      </c>
+      <c r="H21" t="s">
+        <v>293</v>
+      </c>
+      <c r="I21" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>86</v>
       </c>
-      <c r="H12" t="s">
+      <c r="B22" t="s">
         <v>87</v>
       </c>
-      <c r="I12" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="C22" t="s">
+        <v>157</v>
+      </c>
+      <c r="E22" t="s">
+        <v>158</v>
+      </c>
+      <c r="F22" t="s">
+        <v>286</v>
+      </c>
+      <c r="G22" t="s">
+        <v>159</v>
+      </c>
+      <c r="H22" t="s">
+        <v>292</v>
+      </c>
+      <c r="I22" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>88</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B23" t="s">
         <v>89</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C23" t="s">
+        <v>162</v>
+      </c>
+      <c r="E23" t="s">
+        <v>163</v>
+      </c>
+      <c r="F23" t="s">
+        <v>287</v>
+      </c>
+      <c r="G23" t="s">
+        <v>164</v>
+      </c>
+      <c r="H23" t="s">
+        <v>291</v>
+      </c>
+      <c r="I23" t="s">
         <v>165</v>
       </c>
-      <c r="E13" t="s">
-        <v>150</v>
-      </c>
-      <c r="F13" t="s">
-        <v>151</v>
-      </c>
-      <c r="G13" t="s">
-        <v>152</v>
-      </c>
-      <c r="H13" t="s">
-        <v>153</v>
-      </c>
-      <c r="I13" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>90</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B24" t="s">
         <v>91</v>
       </c>
-      <c r="F14" t="s">
-        <v>155</v>
-      </c>
-      <c r="G14" t="s">
-        <v>156</v>
-      </c>
-      <c r="H14" t="s">
-        <v>157</v>
-      </c>
-      <c r="I14" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="C24" t="s">
+        <v>161</v>
+      </c>
+      <c r="E24" t="s">
+        <v>166</v>
+      </c>
+      <c r="F24" t="s">
+        <v>288</v>
+      </c>
+      <c r="G24" t="s">
+        <v>167</v>
+      </c>
+      <c r="H24" t="s">
+        <v>290</v>
+      </c>
+      <c r="I24" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>92</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B25" t="s">
         <v>93</v>
       </c>
-      <c r="C15" t="s">
-        <v>164</v>
-      </c>
-      <c r="E15" t="s">
-        <v>159</v>
-      </c>
-      <c r="F15" t="s">
-        <v>160</v>
-      </c>
-      <c r="G15" t="s">
-        <v>161</v>
-      </c>
-      <c r="H15" t="s">
-        <v>162</v>
-      </c>
-      <c r="I15" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="C25" t="s">
+        <v>169</v>
+      </c>
+      <c r="E25" t="s">
+        <v>170</v>
+      </c>
+      <c r="F25" t="s">
+        <v>171</v>
+      </c>
+      <c r="G25" t="s">
+        <v>172</v>
+      </c>
+      <c r="H25" t="s">
+        <v>173</v>
+      </c>
+      <c r="I25" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>94</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B26" t="s">
         <v>95</v>
       </c>
-      <c r="C16" t="s">
-        <v>166</v>
-      </c>
-      <c r="E16" t="s">
-        <v>167</v>
-      </c>
-      <c r="F16" t="s">
-        <v>168</v>
-      </c>
-      <c r="G16" t="s">
-        <v>169</v>
-      </c>
-      <c r="H16" t="s">
-        <v>170</v>
-      </c>
-      <c r="I16" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="C26" t="s">
+        <v>175</v>
+      </c>
+      <c r="E26" t="s">
+        <v>268</v>
+      </c>
+      <c r="F26" t="s">
+        <v>176</v>
+      </c>
+      <c r="G26" t="s">
+        <v>177</v>
+      </c>
+      <c r="H26" t="s">
+        <v>178</v>
+      </c>
+      <c r="I26" t="s">
         <v>96</v>
       </c>
-      <c r="B17" t="s">
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>97</v>
       </c>
-      <c r="C17" t="s">
-        <v>172</v>
-      </c>
-      <c r="E17" t="s">
-        <v>173</v>
-      </c>
-      <c r="F17" t="s">
-        <v>174</v>
-      </c>
-      <c r="G17" t="s">
-        <v>175</v>
-      </c>
-      <c r="H17" t="s">
-        <v>176</v>
-      </c>
-      <c r="I17" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="B27" t="s">
         <v>98</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C27" t="s">
+        <v>188</v>
+      </c>
+      <c r="E27" t="s">
+        <v>180</v>
+      </c>
+      <c r="F27" t="s">
+        <v>179</v>
+      </c>
+      <c r="G27" t="s">
+        <v>181</v>
+      </c>
+      <c r="H27" t="s">
+        <v>182</v>
+      </c>
+      <c r="I27" t="s">
         <v>99</v>
       </c>
-      <c r="C18" t="s">
-        <v>172</v>
-      </c>
-      <c r="E18" t="s">
-        <v>178</v>
-      </c>
-      <c r="F18" t="s">
-        <v>179</v>
-      </c>
-      <c r="G18" t="s">
-        <v>180</v>
-      </c>
-      <c r="H18" t="s">
-        <v>181</v>
-      </c>
-      <c r="I18" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>100</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B28" t="s">
         <v>101</v>
       </c>
-      <c r="C19" t="s">
-        <v>166</v>
-      </c>
-      <c r="E19" t="s">
+      <c r="C28" t="s">
+        <v>187</v>
+      </c>
+      <c r="E28" t="s">
         <v>183</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F28" t="s">
+        <v>289</v>
+      </c>
+      <c r="G28" t="s">
         <v>184</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H28" t="s">
         <v>185</v>
       </c>
-      <c r="H19" t="s">
+      <c r="I28" t="s">
         <v>186</v>
       </c>
-      <c r="I19" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>102</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B29" t="s">
         <v>103</v>
       </c>
-      <c r="C20" t="s">
-        <v>164</v>
-      </c>
-      <c r="E20" t="s">
-        <v>188</v>
-      </c>
-      <c r="F20" t="s">
+      <c r="C29" t="s">
+        <v>65</v>
+      </c>
+      <c r="E29" t="s">
         <v>189</v>
       </c>
-      <c r="G20" t="s">
+      <c r="F29" t="s">
         <v>190</v>
       </c>
-      <c r="H20" t="s">
+      <c r="G29" t="s">
         <v>191</v>
       </c>
-      <c r="I20" t="s">
+      <c r="H29" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="I29" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>104</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B30" t="s">
         <v>105</v>
       </c>
-      <c r="C21" t="s">
-        <v>193</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="C30" t="s">
         <v>194</v>
       </c>
-      <c r="F21" t="s">
+      <c r="E30" t="s">
         <v>195</v>
       </c>
-      <c r="G21" t="s">
+      <c r="F30" t="s">
         <v>196</v>
       </c>
-      <c r="H21" t="s">
+      <c r="G30" t="s">
         <v>197</v>
       </c>
-      <c r="I21" t="s">
+      <c r="H30" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="I30" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>106</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B31" t="s">
         <v>107</v>
       </c>
-      <c r="C22" t="s">
-        <v>199</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="C31" t="s">
         <v>200</v>
       </c>
-      <c r="F22" t="s">
+      <c r="E31" t="s">
         <v>201</v>
       </c>
-      <c r="G22" t="s">
+      <c r="F31" t="s">
         <v>202</v>
       </c>
-      <c r="H22" t="s">
+      <c r="G31" t="s">
         <v>203</v>
       </c>
-      <c r="I22" t="s">
+      <c r="H31" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="I31" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>108</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B32" t="s">
         <v>109</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C32" t="s">
         <v>206</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E32" t="s">
         <v>207</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F32" t="s">
         <v>208</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G32" t="s">
         <v>209</v>
       </c>
-      <c r="H23" t="s">
+      <c r="H32" t="s">
         <v>210</v>
       </c>
-      <c r="I23" t="s">
+      <c r="I32" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
         <v>110</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B33" t="s">
         <v>111</v>
       </c>
-      <c r="C24" t="s">
-        <v>205</v>
-      </c>
-      <c r="E24" t="s">
+      <c r="C33" t="s">
         <v>212</v>
       </c>
-      <c r="F24" t="s">
+      <c r="E33" t="s">
         <v>213</v>
       </c>
-      <c r="G24" t="s">
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>112</v>
+      </c>
+      <c r="B34" t="s">
+        <v>113</v>
+      </c>
+      <c r="C34" t="s">
+        <v>194</v>
+      </c>
+      <c r="E34" t="s">
+        <v>215</v>
+      </c>
+      <c r="F34" t="s">
+        <v>216</v>
+      </c>
+      <c r="G34" t="s">
+        <v>215</v>
+      </c>
+      <c r="H34" t="s">
+        <v>217</v>
+      </c>
+      <c r="I34" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>114</v>
+      </c>
+      <c r="B35" t="s">
+        <v>115</v>
+      </c>
+      <c r="C35" t="s">
+        <v>194</v>
+      </c>
+      <c r="E35" t="s">
         <v>214</v>
       </c>
-      <c r="H24" t="s">
-        <v>215</v>
-      </c>
-      <c r="I24" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>112</v>
-      </c>
-      <c r="B25" t="s">
-        <v>113</v>
-      </c>
-      <c r="C25" t="s">
-        <v>217</v>
-      </c>
-      <c r="E25" t="s">
-        <v>218</v>
-      </c>
-      <c r="F25" t="s">
+      <c r="F35" t="s">
         <v>219</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G35" t="s">
         <v>220</v>
       </c>
-      <c r="H25" t="s">
+      <c r="H35" t="s">
         <v>221</v>
       </c>
-      <c r="I25" t="s">
+      <c r="I35" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>114</v>
-      </c>
-      <c r="B26" t="s">
-        <v>115</v>
-      </c>
-      <c r="C26" t="s">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>116</v>
+      </c>
+      <c r="B36" t="s">
+        <v>117</v>
+      </c>
+      <c r="C36" t="s">
+        <v>229</v>
+      </c>
+      <c r="E36" t="s">
+        <v>224</v>
+      </c>
+      <c r="F36" t="s">
+        <v>226</v>
+      </c>
+      <c r="G36" t="s">
+        <v>184</v>
+      </c>
+      <c r="H36" t="s">
+        <v>230</v>
+      </c>
+      <c r="I36" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>118</v>
+      </c>
+      <c r="B37" t="s">
+        <v>119</v>
+      </c>
+      <c r="C37" t="s">
         <v>223</v>
       </c>
-      <c r="E26" t="s">
-        <v>224</v>
-      </c>
-      <c r="F26" t="s">
+      <c r="E37" t="s">
         <v>225</v>
       </c>
-      <c r="G26" t="s">
-        <v>226</v>
-      </c>
-      <c r="H26" t="s">
+      <c r="F37" t="s">
+        <v>228</v>
+      </c>
+      <c r="G37" t="s">
         <v>227</v>
       </c>
-      <c r="I26" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>117</v>
-      </c>
-      <c r="B27" t="s">
-        <v>118</v>
-      </c>
-      <c r="C27" t="s">
-        <v>230</v>
-      </c>
-      <c r="E27" t="s">
-        <v>229</v>
-      </c>
-      <c r="F27" t="s">
-        <v>228</v>
-      </c>
-      <c r="G27" t="s">
-        <v>231</v>
-      </c>
-      <c r="H27" t="s">
+      <c r="H37" t="s">
         <v>232</v>
       </c>
-      <c r="I27" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="I37" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
         <v>120</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B38" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="C38" t="s">
+        <v>234</v>
+      </c>
+      <c r="E38" t="s">
+        <v>235</v>
+      </c>
+      <c r="F38" t="s">
+        <v>236</v>
+      </c>
+      <c r="G38" t="s">
+        <v>237</v>
+      </c>
+      <c r="H38" t="s">
+        <v>238</v>
+      </c>
+      <c r="I38" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
         <v>122</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B39" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="C39" t="s">
+        <v>256</v>
+      </c>
+      <c r="E39" t="s">
+        <v>257</v>
+      </c>
+      <c r="F39" t="s">
+        <v>258</v>
+      </c>
+      <c r="G39" t="s">
+        <v>259</v>
+      </c>
+      <c r="H39" t="s">
+        <v>260</v>
+      </c>
+      <c r="I39" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
         <v>124</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B40" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="F40" t="s">
+        <v>240</v>
+      </c>
+      <c r="G40" t="s">
+        <v>241</v>
+      </c>
+      <c r="H40" t="s">
+        <v>242</v>
+      </c>
+      <c r="I40" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
         <v>126</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B41" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="C41" t="s">
+        <v>247</v>
+      </c>
+      <c r="E41" t="s">
+        <v>248</v>
+      </c>
+      <c r="F41" t="s">
+        <v>244</v>
+      </c>
+      <c r="G41" t="s">
+        <v>245</v>
+      </c>
+      <c r="H41" t="s">
+        <v>246</v>
+      </c>
+      <c r="I41" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
         <v>128</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B42" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>130</v>
-      </c>
-      <c r="B33" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>132</v>
-      </c>
-      <c r="B34" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>134</v>
-      </c>
-      <c r="B35" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>136</v>
-      </c>
-      <c r="B36" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>138</v>
-      </c>
-      <c r="B37" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>140</v>
-      </c>
-      <c r="B38" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>142</v>
-      </c>
-      <c r="B39" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>144</v>
-      </c>
-      <c r="B40" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>146</v>
-      </c>
-      <c r="B41" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>148</v>
-      </c>
-      <c r="B42" t="s">
-        <v>149</v>
+      <c r="C42" t="s">
+        <v>250</v>
+      </c>
+      <c r="E42" t="s">
+        <v>251</v>
+      </c>
+      <c r="F42" t="s">
+        <v>252</v>
+      </c>
+      <c r="G42" t="s">
+        <v>253</v>
+      </c>
+      <c r="H42" t="s">
+        <v>254</v>
+      </c>
+      <c r="I42" t="s">
+        <v>255</v>
       </c>
     </row>
   </sheetData>

</xml_diff>